<commit_message>
fixed more players excel stats
</commit_message>
<xml_diff>
--- a/players_stats/Jeff Taylor.xlsx
+++ b/players_stats/Jeff Taylor.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,175 +369,170 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Season</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Season</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Tm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Tm</t>
+          <t>Lg</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Lg</t>
+          <t>Pos</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Pos</t>
+          <t>G</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>GS</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GS</t>
+          <t>MP</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>MP</t>
+          <t>FG</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>FG</t>
+          <t>FGA</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>FGA</t>
+          <t>FG%</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>FG%</t>
+          <t>3P</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>3P</t>
+          <t>3PA</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>3PA</t>
+          <t>3P%</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>3P%</t>
+          <t>2P</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>2P</t>
+          <t>2PA</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>2PA</t>
+          <t>2P%</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>2P%</t>
+          <t>eFG%</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>eFG%</t>
+          <t>FT</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>FT</t>
+          <t>FTA</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>FTA</t>
+          <t>FT%</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>FT%</t>
+          <t>ORB</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>ORB</t>
+          <t>DRB</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>DRB</t>
+          <t>TRB</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>TRB</t>
+          <t>AST</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>BLK</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>BLK</t>
+          <t>TOV</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>TOV</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PTS</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>PTS</t>
+          <t>Height</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Height</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>ShootingHand</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>ShootingHand</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>draftRank</t>
         </is>
@@ -547,364 +542,680 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2012-13</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1982-83</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>23</v>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CHA</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>NBA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NBA</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>44</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" t="n">
-        <v>774</v>
-      </c>
-      <c r="K2" t="n">
-        <v>64</v>
-      </c>
-      <c r="L2" t="n">
-        <v>160</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>64</v>
-      </c>
-      <c r="R2" t="n">
-        <v>159</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.403</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U2" t="n">
-        <v>30</v>
-      </c>
-      <c r="V2" t="n">
-        <v>46</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.652</v>
-      </c>
-      <c r="X2" t="n">
-        <v>25</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>53</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>78</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>110</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>40</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>15</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>60</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>82</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>158</v>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1507</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>172</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>399</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>.431</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>.344</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>245</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>.486</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>.497</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>.728</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>136</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>472</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 201</t>
+        </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 193</t>
+          <t xml:space="preserve"> 102 </t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 79 </t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
           <t>Right</t>
         </is>
       </c>
-      <c r="AJ2" t="n">
-        <v>42</v>
+      <c r="AI2" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2013-14</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1986-87</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>27</v>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHA</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>NBA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>NBA</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>12</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>44</v>
-      </c>
-      <c r="K3" t="n">
-        <v>6</v>
-      </c>
-      <c r="L3" t="n">
-        <v>10</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
-        <v>6</v>
-      </c>
-      <c r="R3" t="n">
-        <v>10</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="U3" t="n">
-        <v>9</v>
-      </c>
-      <c r="V3" t="n">
-        <v>10</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="X3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>21</v>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>218</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>.376</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>.269</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>.424</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>.417</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>.553</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 201</t>
+        </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 193</t>
+          <t xml:space="preserve"> 102 </t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 79 </t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
           <t>Right</t>
         </is>
       </c>
-      <c r="AJ3" t="n">
-        <v>42</v>
+      <c r="AI3" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>2</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2014-15</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CHO</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NBA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>430</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>.395</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>.306</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>.436</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>.443</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>.634</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 201</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 102 </t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="AI4" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Career</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>NBA</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>SG</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>56</v>
-      </c>
-      <c r="I4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J4" t="n">
-        <v>818</v>
-      </c>
-      <c r="K4" t="n">
-        <v>70</v>
-      </c>
-      <c r="L4" t="n">
-        <v>170</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>70</v>
-      </c>
-      <c r="R4" t="n">
-        <v>169</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.414</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.412</v>
-      </c>
-      <c r="U4" t="n">
-        <v>39</v>
-      </c>
-      <c r="V4" t="n">
-        <v>56</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0.696</v>
-      </c>
-      <c r="X4" t="n">
-        <v>26</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>56</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>82</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>113</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>42</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>16</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>68</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>86</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>179</v>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 193</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 79 </t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>132</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2566</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>.409</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>257</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>.319</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>217</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>474</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>.458</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>.465</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>.665</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>263</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>807</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 201</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 102 </t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
         <is>
           <t>Right</t>
         </is>
       </c>
-      <c r="AJ4" t="n">
-        <v>42</v>
+      <c r="AI5" t="n">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>